<commit_message>
Continue Service uses cases
</commit_message>
<xml_diff>
--- a/Q333/UseCases.xlsx
+++ b/Q333/UseCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\Q\Q333\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB832A1-FACC-4999-BDF0-FE7DD7F52F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA5B085-74BA-4442-9342-D86F036D19EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E21B9071-A5A8-4FB8-8334-14FFA2823767}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,13 +82,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -232,10 +244,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -247,17 +260,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,7 +596,7 @@
   <dimension ref="B5:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="F15" sqref="F15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,14 +606,14 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
       <c r="O5">
         <v>2</v>
       </c>
@@ -605,7 +628,7 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="10" t="s">
         <v>0</v>
       </c>
@@ -617,7 +640,7 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>1</v>
       </c>
       <c r="C7" s="1">
@@ -629,18 +652,18 @@
       <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>2</v>
       </c>
       <c r="C8" s="4">
@@ -663,7 +686,7 @@
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>3</v>
       </c>
       <c r="C9" s="4">
@@ -675,18 +698,18 @@
       <c r="E9" s="6">
         <v>3</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="G9" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>4</v>
       </c>
       <c r="C10" s="4">
@@ -709,7 +732,7 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>5</v>
       </c>
       <c r="C11" s="4">
@@ -732,7 +755,7 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>6</v>
       </c>
       <c r="C12" s="4">
@@ -764,7 +787,7 @@
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="14">
+      <c r="B13" s="13">
         <v>7</v>
       </c>
       <c r="C13" s="4">
@@ -776,13 +799,13 @@
       <c r="E13" s="6">
         <v>1</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="23" t="s">
         <v>2</v>
       </c>
       <c r="R13">
@@ -796,7 +819,7 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <v>8</v>
       </c>
       <c r="C14" s="4">
@@ -819,7 +842,7 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="13">
+      <c r="B15" s="12">
         <v>9</v>
       </c>
       <c r="C15" s="7">
@@ -831,18 +854,18 @@
       <c r="E15" s="9">
         <v>3</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="26" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>10</v>
       </c>
       <c r="C16" s="1">
@@ -854,14 +877,14 @@
       <c r="E16" s="3">
         <v>1</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="15" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="14">
+      <c r="B17" s="13">
         <v>11</v>
       </c>
       <c r="C17" s="4">
@@ -873,14 +896,14 @@
       <c r="E17" s="6">
         <v>2</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <v>12</v>
       </c>
       <c r="C18" s="4">
@@ -892,7 +915,7 @@
       <c r="E18" s="6">
         <v>3</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="5"/>
@@ -903,7 +926,7 @@
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="14">
+      <c r="B19" s="13">
         <v>13</v>
       </c>
       <c r="C19" s="4">
@@ -915,14 +938,14 @@
       <c r="E19" s="6">
         <v>1</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="14">
+      <c r="B20" s="13">
         <v>14</v>
       </c>
       <c r="C20" s="4">
@@ -934,14 +957,14 @@
       <c r="E20" s="6">
         <v>2</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="14">
+      <c r="B21" s="13">
         <v>15</v>
       </c>
       <c r="C21" s="4">
@@ -953,14 +976,14 @@
       <c r="E21" s="6">
         <v>3</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="14">
+      <c r="B22" s="13">
         <v>16</v>
       </c>
       <c r="C22" s="4">
@@ -972,14 +995,14 @@
       <c r="E22" s="6">
         <v>1</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="14">
+      <c r="B23" s="13">
         <v>17</v>
       </c>
       <c r="C23" s="4">
@@ -991,14 +1014,14 @@
       <c r="E23" s="6">
         <v>2</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="13">
+      <c r="B24" s="12">
         <v>18</v>
       </c>
       <c r="C24" s="7">
@@ -1010,14 +1033,14 @@
       <c r="E24" s="9">
         <v>3</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="12">
+      <c r="B25" s="11">
         <v>19</v>
       </c>
       <c r="C25" s="1">
@@ -1036,7 +1059,7 @@
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="14">
+      <c r="B26" s="13">
         <v>20</v>
       </c>
       <c r="C26" s="4">
@@ -1055,7 +1078,7 @@
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="14">
+      <c r="B27" s="13">
         <v>21</v>
       </c>
       <c r="C27" s="4">
@@ -1074,7 +1097,7 @@
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="14">
+      <c r="B28" s="13">
         <v>22</v>
       </c>
       <c r="C28" s="4">
@@ -1093,7 +1116,7 @@
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="14">
+      <c r="B29" s="13">
         <v>23</v>
       </c>
       <c r="C29" s="4">
@@ -1112,7 +1135,7 @@
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="14">
+      <c r="B30" s="13">
         <v>24</v>
       </c>
       <c r="C30" s="4">
@@ -1131,7 +1154,7 @@
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="14">
+      <c r="B31" s="13">
         <v>25</v>
       </c>
       <c r="C31" s="4">
@@ -1150,7 +1173,7 @@
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="14">
+      <c r="B32" s="13">
         <v>26</v>
       </c>
       <c r="C32" s="4">
@@ -1169,7 +1192,7 @@
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="13">
+      <c r="B33" s="12">
         <v>27</v>
       </c>
       <c r="C33" s="7">

</xml_diff>